<commit_message>
typo-k javítása, bizonyos adatsorok korrigálása, űrlapon validátor beüzemelése
</commit_message>
<xml_diff>
--- a/data_resource/Database_raw_data.xlsx
+++ b/data_resource/Database_raw_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" state="visible" r:id="rId2"/>
@@ -743,22 +743,22 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +810,7 @@
         <v>315</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>315</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1123,15 +1123,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.9336734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,10 +1626,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,26 +1903,26 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>